<commit_message>
Nova atualização do currículo
</commit_message>
<xml_diff>
--- a/data/cv_entries.xlsx
+++ b/data/cv_entries.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/da4d17bb2dd32c35/Economia/GitHub/alexandrsanches.github.io/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="13_ncr:1_{8635ECF1-BEB6-4883-9DCE-064780583DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C9797D0D-AC3C-4BE4-AC1C-176B17B3C761}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{8635ECF1-BEB6-4883-9DCE-064780583DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EBB7216B-F2A6-4F04-B6E4-F8224FAFBA9A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -149,10 +149,10 @@
     <t>2024 ---</t>
   </si>
   <si>
-    <t>M.Sc. in Economics</t>
-  </si>
-  <si>
     <t>Universidade Católica de Brasília</t>
+  </si>
+  <si>
+    <t>M.Sc. in Economics (in progress)</t>
   </si>
 </sst>
 </file>
@@ -209,6 +209,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -493,7 +497,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -540,10 +544,10 @@
         <v>2024</v>
       </c>
       <c r="D2" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2" t="s">
         <v>38</v>
-      </c>
-      <c r="E2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">

</xml_diff>